<commit_message>
Working, going to change the way the graphs and info frames are displayed. THIS VERSION WORKS BEFORE THE LAYOUT CHANGE.
</commit_message>
<xml_diff>
--- a/RBO_neut.xlsx
+++ b/RBO_neut.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylesmac/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylesmac/PycharmProjects/NIR_ROB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC10F71-A179-8245-A931-4584BCDA14B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF70E20E-6020-3C4A-99B0-CCEA409F9DF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9940" yWindow="2860" windowWidth="18480" windowHeight="14100" activeTab="1" xr2:uid="{4E2D4D2F-6618-1649-9E0A-E42AAD8B8996}"/>
+    <workbookView xWindow="16160" yWindow="2360" windowWidth="18480" windowHeight="14100" activeTab="1" xr2:uid="{4E2D4D2F-6618-1649-9E0A-E42AAD8B8996}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Intensity</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Constant</t>
+  </si>
+  <si>
+    <t>Dark</t>
   </si>
 </sst>
 </file>
@@ -395,2425 +398,3331 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7677CC87-4F26-1F42-B65F-A49C53EECBBC}">
-  <dimension ref="A1:B302"/>
+  <dimension ref="A1:C302"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1350</v>
       </c>
       <c r="B2">
         <v>11172.375</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1351</v>
       </c>
       <c r="B3">
         <v>11133.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1352</v>
       </c>
       <c r="B4">
         <v>11093.320833333333</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1353</v>
       </c>
       <c r="B5">
         <v>11051.65</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1354</v>
       </c>
       <c r="B6">
         <v>11009.316666666666</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1355</v>
       </c>
       <c r="B7">
         <v>10965.324999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1356</v>
       </c>
       <c r="B8">
         <v>10921.062499999996</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1357</v>
       </c>
       <c r="B9">
         <v>10875.508333333337</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1358</v>
       </c>
       <c r="B10">
         <v>10829.174999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1359</v>
       </c>
       <c r="B11">
         <v>10782.170833333332</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1360</v>
       </c>
       <c r="B12">
         <v>10734.512500000003</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1361</v>
       </c>
       <c r="B13">
         <v>10686.537500000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1362</v>
       </c>
       <c r="B14">
         <v>10637.723333333335</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1363</v>
       </c>
       <c r="B15">
         <v>10588.577916666667</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1364</v>
       </c>
       <c r="B16">
         <v>10538.598750000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1365</v>
       </c>
       <c r="B17">
         <v>10487.889583333335</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1366</v>
       </c>
       <c r="B18">
         <v>10436.219999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1367</v>
       </c>
       <c r="B19">
         <v>10383.557500000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1368</v>
       </c>
       <c r="B20">
         <v>10329.945833333331</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1369</v>
       </c>
       <c r="B21">
         <v>10274.922083333335</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1370</v>
       </c>
       <c r="B22">
         <v>10217.450000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1371</v>
       </c>
       <c r="B23">
         <v>10159.460833333334</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1372</v>
       </c>
       <c r="B24">
         <v>10099.384999999998</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1373</v>
       </c>
       <c r="B25">
         <v>10038.137500000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1374</v>
       </c>
       <c r="B26">
         <v>9974.9587499999998</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1375</v>
       </c>
       <c r="B27">
         <v>9910.7616666666672</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1376</v>
       </c>
       <c r="B28">
         <v>9845.6641666666637</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1377</v>
       </c>
       <c r="B29">
         <v>9780.26</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1378</v>
       </c>
       <c r="B30">
         <v>9715.3308333333352</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1379</v>
       </c>
       <c r="B31">
         <v>9650.8708333333307</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1380</v>
       </c>
       <c r="B32">
         <v>9588.4870833333334</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1381</v>
       </c>
       <c r="B33">
         <v>9528.7016666666659</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1382</v>
       </c>
       <c r="B34">
         <v>9472.1450000000023</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1383</v>
       </c>
       <c r="B35">
         <v>9418.9666666666672</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1384</v>
       </c>
       <c r="B36">
         <v>9369.713333333335</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1385</v>
       </c>
       <c r="B37">
         <v>9324.4837500000012</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1386</v>
       </c>
       <c r="B38">
         <v>9283.2308333333331</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1387</v>
       </c>
       <c r="B39">
         <v>9245.712083333332</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1388</v>
       </c>
       <c r="B40">
         <v>9211.3870833333331</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1389</v>
       </c>
       <c r="B41">
         <v>9179.7141666666666</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1390</v>
       </c>
       <c r="B42">
         <v>9150.6562500000018</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1391</v>
       </c>
       <c r="B43">
         <v>9124.4562500000011</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1392</v>
       </c>
       <c r="B44">
         <v>9099.6075000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1393</v>
       </c>
       <c r="B45">
         <v>9076.1970833333326</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1394</v>
       </c>
       <c r="B46">
         <v>9054.820833333335</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1395</v>
       </c>
       <c r="B47">
         <v>9034.4591666666674</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1396</v>
       </c>
       <c r="B48">
         <v>9015.0162499999988</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1397</v>
       </c>
       <c r="B49">
         <v>8996.9154166666649</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1398</v>
       </c>
       <c r="B50">
         <v>8979.0104166666661</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1399</v>
       </c>
       <c r="B51">
         <v>8962.0945833333335</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1400</v>
       </c>
       <c r="B52">
         <v>8945.9483333333337</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1401</v>
       </c>
       <c r="B53">
         <v>8929.8150000000023</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1402</v>
       </c>
       <c r="B54">
         <v>8914.0054166666687</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1403</v>
       </c>
       <c r="B55">
         <v>8898.7241666666669</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1404</v>
       </c>
       <c r="B56">
         <v>8883.3283333333329</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1405</v>
       </c>
       <c r="B57">
         <v>8867.7479166666672</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1406</v>
       </c>
       <c r="B58">
         <v>8852.8379166666673</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1407</v>
       </c>
       <c r="B59">
         <v>8837.567916666665</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1408</v>
       </c>
       <c r="B60">
         <v>8822.2416666666668</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1409</v>
       </c>
       <c r="B61">
         <v>8806.9770833333332</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1410</v>
       </c>
       <c r="B62">
         <v>8792.1854166666653</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1411</v>
       </c>
       <c r="B63">
         <v>8777.2612500000014</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1412</v>
       </c>
       <c r="B64">
         <v>8762.3816666666698</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>1413</v>
       </c>
       <c r="B65">
         <v>8747.6437499999993</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1414</v>
       </c>
       <c r="B66">
         <v>8733.3204166666674</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>1415</v>
       </c>
       <c r="B67">
         <v>8718.6183333333338</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>1416</v>
       </c>
       <c r="B68">
         <v>8704.1020833333332</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>1417</v>
       </c>
       <c r="B69">
         <v>8689.5841666666638</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1418</v>
       </c>
       <c r="B70">
         <v>8674.7945833333342</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>1419</v>
       </c>
       <c r="B71">
         <v>8660.0954166666652</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>1420</v>
       </c>
       <c r="B72">
         <v>8645.4416666666657</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1421</v>
       </c>
       <c r="B73">
         <v>8630.6816666666673</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1422</v>
       </c>
       <c r="B74">
         <v>8616.1924999999992</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>1423</v>
       </c>
       <c r="B75">
         <v>8601.5191666666669</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>1424</v>
       </c>
       <c r="B76">
         <v>8587.2687500000011</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>1425</v>
       </c>
       <c r="B77">
         <v>8573.1600000000017</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>1426</v>
       </c>
       <c r="B78">
         <v>8559.3924999999999</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>1427</v>
       </c>
       <c r="B79">
         <v>8545.9083333333347</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1428</v>
       </c>
       <c r="B80">
         <v>8532.8808333333345</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1429</v>
       </c>
       <c r="B81">
         <v>8520.3362500000003</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1430</v>
       </c>
       <c r="B82">
         <v>8507.9054166666665</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1431</v>
       </c>
       <c r="B83">
         <v>8495.7104166666668</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1432</v>
       </c>
       <c r="B84">
         <v>8484.0562499999996</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1433</v>
       </c>
       <c r="B85">
         <v>8472.0079166666656</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1434</v>
       </c>
       <c r="B86">
         <v>8460.4874999999993</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1435</v>
       </c>
       <c r="B87">
         <v>8449.0837499999998</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>1436</v>
       </c>
       <c r="B88">
         <v>8437.7245833333309</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1437</v>
       </c>
       <c r="B89">
         <v>8426.8958333333339</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>1438</v>
       </c>
       <c r="B90">
         <v>8415.9141666666656</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>1439</v>
       </c>
       <c r="B91">
         <v>8405.3412500000013</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>1440</v>
       </c>
       <c r="B92">
         <v>8394.92</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>1441</v>
       </c>
       <c r="B93">
         <v>8384.690833333334</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>1442</v>
       </c>
       <c r="B94">
         <v>8374.3616666666658</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>1443</v>
       </c>
       <c r="B95">
         <v>8363.9908333333315</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>1444</v>
       </c>
       <c r="B96">
         <v>8353.52</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>1445</v>
       </c>
       <c r="B97">
         <v>8343.5183333333334</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>1446</v>
       </c>
       <c r="B98">
         <v>8333.3850000000002</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>1447</v>
       </c>
       <c r="B99">
         <v>8323.5062500000004</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>1448</v>
       </c>
       <c r="B100">
         <v>8313.8533333333344</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>1449</v>
       </c>
       <c r="B101">
         <v>8304.3912500000006</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>1450</v>
       </c>
       <c r="B102">
         <v>8295.152916666666</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>1451</v>
       </c>
       <c r="B103">
         <v>8285.8320833333346</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>1452</v>
       </c>
       <c r="B104">
         <v>8277.0333333333347</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>1453</v>
       </c>
       <c r="B105">
         <v>8268.0849999999991</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>1454</v>
       </c>
       <c r="B106">
         <v>8259.5750000000007</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>1455</v>
       </c>
       <c r="B107">
         <v>8251.4408333333322</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>1456</v>
       </c>
       <c r="B108">
         <v>8243.3491666666687</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>1457</v>
       </c>
       <c r="B109">
         <v>8235.5808333333334</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>1458</v>
       </c>
       <c r="B110">
         <v>8227.6162499999991</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>1459</v>
       </c>
       <c r="B111">
         <v>8220.1558333333323</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>1460</v>
       </c>
       <c r="B112">
         <v>8212.4091666666664</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>1461</v>
       </c>
       <c r="B113">
         <v>8204.9362500000007</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>1462</v>
       </c>
       <c r="B114">
         <v>8197.3608333333341</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>1463</v>
       </c>
       <c r="B115">
         <v>8189.7150000000001</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>1464</v>
       </c>
       <c r="B116">
         <v>8182.2645833333336</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>1465</v>
       </c>
       <c r="B117">
         <v>8174.8920833333332</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>1466</v>
       </c>
       <c r="B118">
         <v>8167.8029166666674</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>1467</v>
       </c>
       <c r="B119">
         <v>8160.8950000000004</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>1468</v>
       </c>
       <c r="B120">
         <v>8154.3104166666672</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>1469</v>
       </c>
       <c r="B121">
         <v>8147.866666666665</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>1470</v>
       </c>
       <c r="B122">
         <v>8141.9604166666686</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>1471</v>
       </c>
       <c r="B123">
         <v>8135.902916666666</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>1472</v>
       </c>
       <c r="B124">
         <v>8130.6433333333343</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>1473</v>
       </c>
       <c r="B125">
         <v>8125.350833333333</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>1474</v>
       </c>
       <c r="B126">
         <v>8120.5166666666655</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>1475</v>
       </c>
       <c r="B127">
         <v>8115.9174999999996</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>1476</v>
       </c>
       <c r="B128">
         <v>8111.4425000000001</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>1477</v>
       </c>
       <c r="B129">
         <v>8106.9204166666668</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>1478</v>
       </c>
       <c r="B130">
         <v>8103.005000000001</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>1479</v>
       </c>
       <c r="B131">
         <v>8099.0837500000016</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>1480</v>
       </c>
       <c r="B132">
         <v>8095.3395833333343</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>1481</v>
       </c>
       <c r="B133">
         <v>8091.8020833333321</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>1482</v>
       </c>
       <c r="B134">
         <v>8088.0283333333346</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>1483</v>
       </c>
       <c r="B135">
         <v>8084.7929166666654</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>1484</v>
       </c>
       <c r="B136">
         <v>8081.3112499999997</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>1485</v>
       </c>
       <c r="B137">
         <v>8078.0583333333334</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>1486</v>
       </c>
       <c r="B138">
         <v>8075.1112500000008</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>1487</v>
       </c>
       <c r="B139">
         <v>8072.0875000000005</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>1488</v>
       </c>
       <c r="B140">
         <v>8069.4191666666657</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>1489</v>
       </c>
       <c r="B141">
         <v>8066.8295833333314</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>1490</v>
       </c>
       <c r="B142">
         <v>8064.3808333333336</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>1491</v>
       </c>
       <c r="B143">
         <v>8062.213749999999</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>1492</v>
       </c>
       <c r="B144">
         <v>8060.430000000003</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>1493</v>
       </c>
       <c r="B145">
         <v>8058.4308333333329</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>1494</v>
       </c>
       <c r="B146">
         <v>8056.588749999999</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>1495</v>
       </c>
       <c r="B147">
         <v>8054.827916666668</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>1496</v>
       </c>
       <c r="B148">
         <v>8053.421666666668</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>1497</v>
       </c>
       <c r="B149">
         <v>8051.9658333333355</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>1498</v>
       </c>
       <c r="B150">
         <v>8051.1045833333346</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>1499</v>
       </c>
       <c r="B151">
         <v>8050.6091666666662</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>1500</v>
       </c>
       <c r="B152">
         <v>8050.5445833333315</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>1501</v>
       </c>
       <c r="B153">
         <v>8050.6037500000011</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>1502</v>
       </c>
       <c r="B154">
         <v>8050.8720833333327</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>1503</v>
       </c>
       <c r="B155">
         <v>8051.7087500000016</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>1504</v>
       </c>
       <c r="B156">
         <v>8052.5595833333318</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>1505</v>
       </c>
       <c r="B157">
         <v>8053.4608333333317</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>1506</v>
       </c>
       <c r="B158">
         <v>8054.2008333333333</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>1507</v>
       </c>
       <c r="B159">
         <v>8055.2833333333356</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>1508</v>
       </c>
       <c r="B160">
         <v>8056.4616666666661</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>1509</v>
       </c>
       <c r="B161">
         <v>8057.6466666666674</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>1510</v>
       </c>
       <c r="B162">
         <v>8059.2750000000015</v>
       </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>1511</v>
       </c>
       <c r="B163">
         <v>8060.7029166666662</v>
       </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>1512</v>
       </c>
       <c r="B164">
         <v>8062.0595833333318</v>
       </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>1513</v>
       </c>
       <c r="B165">
         <v>8063.4745833333327</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>1514</v>
       </c>
       <c r="B166">
         <v>8065.4445833333339</v>
       </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>1515</v>
       </c>
       <c r="B167">
         <v>8067.0945833333353</v>
       </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>1516</v>
       </c>
       <c r="B168">
         <v>8069.2954166666668</v>
       </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>1517</v>
       </c>
       <c r="B169">
         <v>8071.8566666666675</v>
       </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>1518</v>
       </c>
       <c r="B170">
         <v>8074.5704166666656</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>1519</v>
       </c>
       <c r="B171">
         <v>8077.8437500000009</v>
       </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>1520</v>
       </c>
       <c r="B172">
         <v>8081.4941666666682</v>
       </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>1521</v>
       </c>
       <c r="B173">
         <v>8084.9712499999996</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>1522</v>
       </c>
       <c r="B174">
         <v>8089.097083333334</v>
       </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>1523</v>
       </c>
       <c r="B175">
         <v>8093.0258333333331</v>
       </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>1524</v>
       </c>
       <c r="B176">
         <v>8096.7579166666683</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>1525</v>
       </c>
       <c r="B177">
         <v>8100.9800000000023</v>
       </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>1526</v>
       </c>
       <c r="B178">
         <v>8104.8666666666677</v>
       </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>1527</v>
       </c>
       <c r="B179">
         <v>8109.4354166666681</v>
       </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>1528</v>
       </c>
       <c r="B180">
         <v>8113.743333333332</v>
       </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>1529</v>
       </c>
       <c r="B181">
         <v>8118.2949999999992</v>
       </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>1530</v>
       </c>
       <c r="B182">
         <v>8123.0383333333302</v>
       </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>1531</v>
       </c>
       <c r="B183">
         <v>8127.6287499999999</v>
       </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>1532</v>
       </c>
       <c r="B184">
         <v>8132.8149999999996</v>
       </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>1533</v>
       </c>
       <c r="B185">
         <v>8138.1933333333336</v>
       </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>1534</v>
       </c>
       <c r="B186">
         <v>8143.6520833333343</v>
       </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>1535</v>
       </c>
       <c r="B187">
         <v>8149.5433333333322</v>
       </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>1536</v>
       </c>
       <c r="B188">
         <v>8155.5750000000007</v>
       </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>1537</v>
       </c>
       <c r="B189">
         <v>8161.8833333333341</v>
       </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>1538</v>
       </c>
       <c r="B190">
         <v>8168.1104166666655</v>
       </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>1539</v>
       </c>
       <c r="B191">
         <v>8174.5129166666693</v>
       </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>1540</v>
       </c>
       <c r="B192">
         <v>8181.6987499999996</v>
       </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>1541</v>
       </c>
       <c r="B193">
         <v>8188.3208333333314</v>
       </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>1542</v>
       </c>
       <c r="B194">
         <v>8195.1679166666672</v>
       </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>1543</v>
       </c>
       <c r="B195">
         <v>8202.4191666666648</v>
       </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>1544</v>
       </c>
       <c r="B196">
         <v>8209.3595833333329</v>
       </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>1545</v>
       </c>
       <c r="B197">
         <v>8216.6437500000011</v>
       </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>1546</v>
       </c>
       <c r="B198">
         <v>8224.4470833333307</v>
       </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>1547</v>
       </c>
       <c r="B199">
         <v>8231.9795833333319</v>
       </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>1548</v>
       </c>
       <c r="B200">
         <v>8239.937083333336</v>
       </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>1549</v>
       </c>
       <c r="B201">
         <v>8247.6874999999982</v>
       </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>1550</v>
       </c>
       <c r="B202">
         <v>8255.9270833333303</v>
       </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>1551</v>
       </c>
       <c r="B203">
         <v>8264.2525000000005</v>
       </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>1552</v>
       </c>
       <c r="B204">
         <v>8272.876666666667</v>
       </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>1553</v>
       </c>
       <c r="B205">
         <v>8281.6075000000001</v>
       </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>1554</v>
       </c>
       <c r="B206">
         <v>8290.6983333333319</v>
       </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>1555</v>
       </c>
       <c r="B207">
         <v>8299.7862499999992</v>
       </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>1556</v>
       </c>
       <c r="B208">
         <v>8309.1683333333331</v>
       </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>1557</v>
       </c>
       <c r="B209">
         <v>8318.6283333333322</v>
       </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>1558</v>
       </c>
       <c r="B210">
         <v>8328.3558333333331</v>
       </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>1559</v>
       </c>
       <c r="B211">
         <v>8338.4579166666663</v>
       </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>1560</v>
       </c>
       <c r="B212">
         <v>8348.5541666666668</v>
       </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>1561</v>
       </c>
       <c r="B213">
         <v>8358.600416666668</v>
       </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>1562</v>
       </c>
       <c r="B214">
         <v>8368.7070833333328</v>
       </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>1563</v>
       </c>
       <c r="B215">
         <v>8378.5624999999982</v>
       </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>1564</v>
       </c>
       <c r="B216">
         <v>8388.6750000000011</v>
       </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>1565</v>
       </c>
       <c r="B217">
         <v>8398.8325000000004</v>
       </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>1566</v>
       </c>
       <c r="B218">
         <v>8409.154166666669</v>
       </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>1567</v>
       </c>
       <c r="B219">
         <v>8419.9162500000002</v>
       </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>1568</v>
       </c>
       <c r="B220">
         <v>8430.9066666666677</v>
       </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>1569</v>
       </c>
       <c r="B221">
         <v>8441.7816666666658</v>
       </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>1570</v>
       </c>
       <c r="B222">
         <v>8453.3291666666682</v>
       </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>1571</v>
       </c>
       <c r="B223">
         <v>8465.463333333335</v>
       </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>1572</v>
       </c>
       <c r="B224">
         <v>8477.4879166666669</v>
       </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>1573</v>
       </c>
       <c r="B225">
         <v>8489.6841666666642</v>
       </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>1574</v>
       </c>
       <c r="B226">
         <v>8502.3700000000008</v>
       </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>1575</v>
       </c>
       <c r="B227">
         <v>8515.0445833333324</v>
       </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>1576</v>
       </c>
       <c r="B228">
         <v>8527.7708333333321</v>
       </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>1577</v>
       </c>
       <c r="B229">
         <v>8540.6225000000031</v>
       </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>1578</v>
       </c>
       <c r="B230">
         <v>8553.6470833333351</v>
       </c>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>1579</v>
       </c>
       <c r="B231">
         <v>8566.5524999999998</v>
       </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>1580</v>
       </c>
       <c r="B232">
         <v>8579.7112500000021</v>
       </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>1581</v>
       </c>
       <c r="B233">
         <v>8592.992916666668</v>
       </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>1582</v>
       </c>
       <c r="B234">
         <v>8606.3016666666645</v>
       </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>1583</v>
       </c>
       <c r="B235">
         <v>8619.4708333333328</v>
       </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>1584</v>
       </c>
       <c r="B236">
         <v>8632.6762499999986</v>
       </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>1585</v>
       </c>
       <c r="B237">
         <v>8645.9308333333302</v>
       </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>1586</v>
       </c>
       <c r="B238">
         <v>8659.3904166666634</v>
       </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>1587</v>
       </c>
       <c r="B239">
         <v>8673.3854166666661</v>
       </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>1588</v>
       </c>
       <c r="B240">
         <v>8687.2912500000002</v>
       </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>1589</v>
       </c>
       <c r="B241">
         <v>8701.5220833333333</v>
       </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>1590</v>
       </c>
       <c r="B242">
         <v>8715.9704166666652</v>
       </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>1591</v>
       </c>
       <c r="B243">
         <v>8730.9445833333339</v>
       </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C243">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>1592</v>
       </c>
       <c r="B244">
         <v>8746.0979166666675</v>
       </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C244">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>1593</v>
       </c>
       <c r="B245">
         <v>8761.8304166666694</v>
       </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>1594</v>
       </c>
       <c r="B246">
         <v>8777.4254166666688</v>
       </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>1595</v>
       </c>
       <c r="B247">
         <v>8793.1624999999985</v>
       </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>1596</v>
       </c>
       <c r="B248">
         <v>8809.3570833333342</v>
       </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>1597</v>
       </c>
       <c r="B249">
         <v>8825.5808333333334</v>
       </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>1598</v>
       </c>
       <c r="B250">
         <v>8841.6762500000004</v>
       </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>1599</v>
       </c>
       <c r="B251">
         <v>8857.8958333333339</v>
       </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C251">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>1600</v>
       </c>
       <c r="B252">
         <v>8874.3445833333335</v>
       </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>1601</v>
       </c>
       <c r="B253">
         <v>8890.585416666665</v>
       </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C253">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>1602</v>
       </c>
       <c r="B254">
         <v>8907.2287500000002</v>
       </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C254">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>1603</v>
       </c>
       <c r="B255">
         <v>8923.901249999999</v>
       </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>1604</v>
       </c>
       <c r="B256">
         <v>8940.8079166666666</v>
       </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C256">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>1605</v>
       </c>
       <c r="B257">
         <v>8957.9187500000007</v>
       </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>1606</v>
       </c>
       <c r="B258">
         <v>8975.0187500000011</v>
       </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>1607</v>
       </c>
       <c r="B259">
         <v>8991.8016666666663</v>
       </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C259">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>1608</v>
       </c>
       <c r="B260">
         <v>9008.6216666666678</v>
       </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C260">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>1609</v>
       </c>
       <c r="B261">
         <v>9025.7308333333331</v>
       </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C261">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>1610</v>
       </c>
       <c r="B262">
         <v>9042.7008333333342</v>
       </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C262">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>1611</v>
       </c>
       <c r="B263">
         <v>9059.6845833333336</v>
       </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C263">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>1612</v>
       </c>
       <c r="B264">
         <v>9077.0562499999996</v>
       </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C264">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>1613</v>
       </c>
       <c r="B265">
         <v>9094.2616666666672</v>
       </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C265">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>1614</v>
       </c>
       <c r="B266">
         <v>9111.8687500000033</v>
       </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C266">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>1615</v>
       </c>
       <c r="B267">
         <v>9129.6608333333334</v>
       </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C267">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>1616</v>
       </c>
       <c r="B268">
         <v>9147.7274999999991</v>
       </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C268">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>1617</v>
       </c>
       <c r="B269">
         <v>9166.0374999999985</v>
       </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C269">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>1618</v>
       </c>
       <c r="B270">
         <v>9184.2766666666666</v>
       </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C270">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>1619</v>
       </c>
       <c r="B271">
         <v>9202.8912500000024</v>
       </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C271">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>1620</v>
       </c>
       <c r="B272">
         <v>9221.159583333334</v>
       </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C272">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>1621</v>
       </c>
       <c r="B273">
         <v>9239.8941666666669</v>
       </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>1622</v>
       </c>
       <c r="B274">
         <v>9258.1991666666636</v>
       </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C274">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>1623</v>
       </c>
       <c r="B275">
         <v>9277.2554166666669</v>
       </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C275">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>1624</v>
       </c>
       <c r="B276">
         <v>9295.6841666666678</v>
       </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C276">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>1625</v>
       </c>
       <c r="B277">
         <v>9314.5687500000004</v>
       </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C277">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>1626</v>
       </c>
       <c r="B278">
         <v>9333.2699999999986</v>
       </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C278">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>1627</v>
       </c>
       <c r="B279">
         <v>9351.972083333334</v>
       </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C279">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>1628</v>
       </c>
       <c r="B280">
         <v>9370.8737500000025</v>
       </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>1629</v>
       </c>
       <c r="B281">
         <v>9389.4283333333315</v>
       </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C281">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>1630</v>
       </c>
       <c r="B282">
         <v>9408.522916666665</v>
       </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C282">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>1631</v>
       </c>
       <c r="B283">
         <v>9427.6933333333345</v>
       </c>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C283">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>1632</v>
       </c>
       <c r="B284">
         <v>9446.7300000000014</v>
       </c>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>1633</v>
       </c>
       <c r="B285">
         <v>9466.1470833333351</v>
       </c>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C285">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>1634</v>
       </c>
       <c r="B286">
         <v>9485.6054166666672</v>
       </c>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C286">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>1635</v>
       </c>
       <c r="B287">
         <v>9504.838333333335</v>
       </c>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C287">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>1636</v>
       </c>
       <c r="B288">
         <v>9524.3841666666649</v>
       </c>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>1637</v>
       </c>
       <c r="B289">
         <v>9543.7066666666633</v>
       </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>1638</v>
       </c>
       <c r="B290">
         <v>9562.9254166666669</v>
       </c>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>1639</v>
       </c>
       <c r="B291">
         <v>9582.1083333333354</v>
       </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>1640</v>
       </c>
       <c r="B292">
         <v>9601.2250000000022</v>
       </c>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>1641</v>
       </c>
       <c r="B293">
         <v>9620.1249999999982</v>
       </c>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>1642</v>
       </c>
       <c r="B294">
         <v>9639.0512500000004</v>
       </c>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>1643</v>
       </c>
       <c r="B295">
         <v>9657.7054166666658</v>
       </c>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>1644</v>
       </c>
       <c r="B296">
         <v>9676.7316666666684</v>
       </c>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C296">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>1645</v>
       </c>
       <c r="B297">
         <v>9694.9916666666668</v>
       </c>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>1646</v>
       </c>
       <c r="B298">
         <v>9713.7091666666674</v>
       </c>
-    </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>1647</v>
       </c>
       <c r="B299">
         <v>9732.4583333333339</v>
       </c>
-    </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C299">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>1648</v>
       </c>
       <c r="B300">
         <v>9751.3341666666693</v>
       </c>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>1649</v>
       </c>
       <c r="B301">
         <v>9770.1366666666672</v>
       </c>
-    </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>1650</v>
       </c>
       <c r="B302">
         <v>9789.1095833333329</v>
+      </c>
+      <c r="C302">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2826,7 +3735,7 @@
   <dimension ref="A1:B303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B303" sqref="B303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>